<commit_message>
Add the total aggregated column
Total aggregated column is added in the data, see spillover folder for details  

Tasks: 1. check the spillover analysis 2. conduct scenario forecasting .
</commit_message>
<xml_diff>
--- a/Matlab/ABSemp.xlsx
+++ b/Matlab/ABSemp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elvisyang/Desktop/hon_proj/Sectoral Employment/Spilover/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elvisyang/Desktop/hon_proj/Disaggregated_Employment/Matlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FDA202-CD42-164E-9E98-3310229D39FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480ABB09-C2F0-9F4B-A591-4146F3D79F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37260" yWindow="500" windowWidth="37260" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="two_digit_data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>01 Agriculture</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t xml:space="preserve">95 Personal and other services (include activities for own use) </t>
+  </si>
+  <si>
+    <t>96 Total</t>
   </si>
 </sst>
 </file>
@@ -791,7 +794,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -803,6 +806,7 @@
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1160,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CK153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BJ1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="BV9" sqref="BV9"/>
+    <sheetView tabSelected="1" topLeftCell="BV1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="CG2" sqref="CG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1423,6 +1427,9 @@
       <c r="CF1" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="CG1" s="3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="2" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
@@ -1677,6 +1684,9 @@
       <c r="CF2" s="4">
         <v>124.79241590000001</v>
       </c>
+      <c r="CG2" s="7">
+        <v>6576.0618182999997</v>
+      </c>
     </row>
     <row r="3" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
@@ -1930,6 +1940,9 @@
       </c>
       <c r="CF3" s="4">
         <v>123.19022219999999</v>
+      </c>
+      <c r="CG3" s="7">
+        <v>6595.6641925000004</v>
       </c>
       <c r="CK3" s="1"/>
     </row>
@@ -2186,6 +2199,9 @@
       <c r="CF4" s="4">
         <v>121.69017589999999</v>
       </c>
+      <c r="CG4" s="7">
+        <v>6657.9327706000004</v>
+      </c>
       <c r="CK4" s="1"/>
     </row>
     <row r="5" spans="1:89" x14ac:dyDescent="0.2">
@@ -2441,6 +2457,9 @@
       <c r="CF5" s="4">
         <v>119.53997770000001</v>
       </c>
+      <c r="CG5" s="7">
+        <v>6675.5378567999996</v>
+      </c>
       <c r="CK5" s="1"/>
     </row>
     <row r="6" spans="1:89" x14ac:dyDescent="0.2">
@@ -2696,6 +2715,9 @@
       <c r="CF6" s="4">
         <v>128.32108290000002</v>
       </c>
+      <c r="CG6" s="7">
+        <v>6881.9441951999997</v>
+      </c>
       <c r="CK6" s="1"/>
     </row>
     <row r="7" spans="1:89" x14ac:dyDescent="0.2">
@@ -2951,6 +2973,9 @@
       <c r="CF7" s="4">
         <v>129.57616059999998</v>
       </c>
+      <c r="CG7" s="7">
+        <v>6861.8554940000004</v>
+      </c>
       <c r="CK7" s="1"/>
     </row>
     <row r="8" spans="1:89" x14ac:dyDescent="0.2">
@@ -3206,6 +3231,9 @@
       <c r="CF8" s="4">
         <v>132.38833460000001</v>
       </c>
+      <c r="CG8" s="7">
+        <v>6978.9699757999997</v>
+      </c>
       <c r="CK8" s="1"/>
     </row>
     <row r="9" spans="1:89" x14ac:dyDescent="0.2">
@@ -3461,6 +3489,9 @@
       <c r="CF9" s="4">
         <v>127.945267</v>
       </c>
+      <c r="CG9" s="7">
+        <v>6918.5250524000003</v>
+      </c>
       <c r="CK9" s="1"/>
     </row>
     <row r="10" spans="1:89" x14ac:dyDescent="0.2">
@@ -3716,6 +3747,9 @@
       <c r="CF10" s="4">
         <v>136.098702</v>
       </c>
+      <c r="CG10" s="7">
+        <v>7034.1639395000002</v>
+      </c>
       <c r="CK10" s="1"/>
     </row>
     <row r="11" spans="1:89" x14ac:dyDescent="0.2">
@@ -3971,6 +4005,9 @@
       <c r="CF11" s="4">
         <v>135.91628109999999</v>
       </c>
+      <c r="CG11" s="7">
+        <v>7022.2527528999999</v>
+      </c>
       <c r="CK11" s="1"/>
     </row>
     <row r="12" spans="1:89" x14ac:dyDescent="0.2">
@@ -4226,6 +4263,9 @@
       <c r="CF12" s="4">
         <v>141.59997849999999</v>
       </c>
+      <c r="CG12" s="7">
+        <v>7103.5234570000002</v>
+      </c>
       <c r="CK12" s="1"/>
     </row>
     <row r="13" spans="1:89" x14ac:dyDescent="0.2">
@@ -4481,6 +4521,9 @@
       <c r="CF13" s="4">
         <v>147.2182664</v>
       </c>
+      <c r="CG13" s="7">
+        <v>7092.2573214000004</v>
+      </c>
       <c r="CK13" s="1"/>
     </row>
     <row r="14" spans="1:89" x14ac:dyDescent="0.2">
@@ -4736,6 +4779,9 @@
       <c r="CF14" s="4">
         <v>146.7248386</v>
       </c>
+      <c r="CG14" s="7">
+        <v>7182.1613009000002</v>
+      </c>
       <c r="CK14" s="1"/>
     </row>
     <row r="15" spans="1:89" x14ac:dyDescent="0.2">
@@ -4991,6 +5037,9 @@
       <c r="CF15" s="4">
         <v>149.90515590000001</v>
       </c>
+      <c r="CG15" s="7">
+        <v>7247.3043494000003</v>
+      </c>
       <c r="CK15" s="1"/>
     </row>
     <row r="16" spans="1:89" x14ac:dyDescent="0.2">
@@ -5246,6 +5295,9 @@
       <c r="CF16" s="4">
         <v>150.961298</v>
       </c>
+      <c r="CG16" s="7">
+        <v>7354.8338311999996</v>
+      </c>
       <c r="CK16" s="1"/>
     </row>
     <row r="17" spans="1:89" x14ac:dyDescent="0.2">
@@ -5501,6 +5553,9 @@
       <c r="CF17" s="4">
         <v>152.3169082</v>
       </c>
+      <c r="CG17" s="7">
+        <v>7353.2863914999998</v>
+      </c>
       <c r="CK17" s="1"/>
     </row>
     <row r="18" spans="1:89" x14ac:dyDescent="0.2">
@@ -5756,6 +5811,9 @@
       <c r="CF18" s="4">
         <v>155.54561320000002</v>
       </c>
+      <c r="CG18" s="7">
+        <v>7508.606914</v>
+      </c>
       <c r="CK18" s="1"/>
     </row>
     <row r="19" spans="1:89" x14ac:dyDescent="0.2">
@@ -6011,6 +6069,9 @@
       <c r="CF19" s="4">
         <v>140.26626970000001</v>
       </c>
+      <c r="CG19" s="7">
+        <v>7566.4884234000001</v>
+      </c>
       <c r="CK19" s="1"/>
     </row>
     <row r="20" spans="1:89" x14ac:dyDescent="0.2">
@@ -6266,6 +6327,9 @@
       <c r="CF20" s="4">
         <v>147.216757</v>
       </c>
+      <c r="CG20" s="7">
+        <v>7720.7895072000001</v>
+      </c>
       <c r="CK20" s="1"/>
     </row>
     <row r="21" spans="1:89" x14ac:dyDescent="0.2">
@@ -6521,6 +6585,9 @@
       <c r="CF21" s="4">
         <v>146.5428058</v>
       </c>
+      <c r="CG21" s="7">
+        <v>7715.2730129000001</v>
+      </c>
       <c r="CK21" s="1"/>
     </row>
     <row r="22" spans="1:89" x14ac:dyDescent="0.2">
@@ -6776,6 +6843,9 @@
       <c r="CF22" s="4">
         <v>158.35764370000001</v>
       </c>
+      <c r="CG22" s="7">
+        <v>7862.3568226999996</v>
+      </c>
       <c r="CK22" s="1"/>
     </row>
     <row r="23" spans="1:89" x14ac:dyDescent="0.2">
@@ -7031,6 +7101,9 @@
       <c r="CF23" s="4">
         <v>152.2173707</v>
       </c>
+      <c r="CG23" s="7">
+        <v>7802.9902621000001</v>
+      </c>
       <c r="CK23" s="1"/>
     </row>
     <row r="24" spans="1:89" x14ac:dyDescent="0.2">
@@ -7286,6 +7359,9 @@
       <c r="CF24" s="4">
         <v>156.4768742</v>
       </c>
+      <c r="CG24" s="7">
+        <v>7908.4636763999997</v>
+      </c>
       <c r="CK24" s="1"/>
     </row>
     <row r="25" spans="1:89" x14ac:dyDescent="0.2">
@@ -7541,6 +7617,9 @@
       <c r="CF25" s="4">
         <v>146.8285013</v>
       </c>
+      <c r="CG25" s="7">
+        <v>7807.9828870000001</v>
+      </c>
       <c r="CK25" s="1"/>
     </row>
     <row r="26" spans="1:89" x14ac:dyDescent="0.2">
@@ -7796,6 +7875,9 @@
       <c r="CF26" s="4">
         <v>153.72913130000001</v>
       </c>
+      <c r="CG26" s="7">
+        <v>7826.9227229999997</v>
+      </c>
       <c r="CK26" s="1"/>
     </row>
     <row r="27" spans="1:89" x14ac:dyDescent="0.2">
@@ -8051,6 +8133,9 @@
       <c r="CF27" s="4">
         <v>151.6467705</v>
       </c>
+      <c r="CG27" s="7">
+        <v>7708.7805939</v>
+      </c>
       <c r="CK27" s="1"/>
     </row>
     <row r="28" spans="1:89" x14ac:dyDescent="0.2">
@@ -8306,6 +8391,9 @@
       <c r="CF28" s="4">
         <v>158.31951379999998</v>
       </c>
+      <c r="CG28" s="7">
+        <v>7703.7164486000001</v>
+      </c>
       <c r="CK28" s="1"/>
     </row>
     <row r="29" spans="1:89" x14ac:dyDescent="0.2">
@@ -8561,6 +8649,9 @@
       <c r="CF29" s="4">
         <v>153.38029750000001</v>
       </c>
+      <c r="CG29" s="7">
+        <v>7620.7032112999996</v>
+      </c>
       <c r="CK29" s="1"/>
     </row>
     <row r="30" spans="1:89" x14ac:dyDescent="0.2">
@@ -8816,6 +8907,9 @@
       <c r="CF30" s="4">
         <v>157.9798175</v>
       </c>
+      <c r="CG30" s="7">
+        <v>7614.9417599999997</v>
+      </c>
       <c r="CK30" s="1"/>
     </row>
     <row r="31" spans="1:89" x14ac:dyDescent="0.2">
@@ -9071,6 +9165,9 @@
       <c r="CF31" s="4">
         <v>172.1036794</v>
       </c>
+      <c r="CG31" s="7">
+        <v>7597.1754529999998</v>
+      </c>
       <c r="CK31" s="1"/>
     </row>
     <row r="32" spans="1:89" x14ac:dyDescent="0.2">
@@ -9326,6 +9423,9 @@
       <c r="CF32" s="4">
         <v>175.84170260000002</v>
       </c>
+      <c r="CG32" s="7">
+        <v>7631.4000545999997</v>
+      </c>
       <c r="CK32" s="1"/>
     </row>
     <row r="33" spans="1:89" x14ac:dyDescent="0.2">
@@ -9581,6 +9681,9 @@
       <c r="CF33" s="4">
         <v>177.04970279999998</v>
       </c>
+      <c r="CG33" s="7">
+        <v>7613.3991011999997</v>
+      </c>
       <c r="CK33" s="1"/>
     </row>
     <row r="34" spans="1:89" x14ac:dyDescent="0.2">
@@ -9836,6 +9939,9 @@
       <c r="CF34" s="4">
         <v>163.40153840000002</v>
       </c>
+      <c r="CG34" s="7">
+        <v>7587.4465005000002</v>
+      </c>
       <c r="CK34" s="1"/>
     </row>
     <row r="35" spans="1:89" x14ac:dyDescent="0.2">
@@ -10091,6 +10197,9 @@
       <c r="CF35" s="4">
         <v>162.635829</v>
       </c>
+      <c r="CG35" s="7">
+        <v>7530.9593086000004</v>
+      </c>
       <c r="CK35" s="1"/>
     </row>
     <row r="36" spans="1:89" x14ac:dyDescent="0.2">
@@ -10346,6 +10455,9 @@
       <c r="CF36" s="4">
         <v>164.5183084</v>
       </c>
+      <c r="CG36" s="7">
+        <v>7620.5067890999999</v>
+      </c>
       <c r="CK36" s="1"/>
     </row>
     <row r="37" spans="1:89" x14ac:dyDescent="0.2">
@@ -10601,6 +10713,9 @@
       <c r="CF37" s="4">
         <v>155.3013641</v>
       </c>
+      <c r="CG37" s="7">
+        <v>7589.4031314000003</v>
+      </c>
       <c r="CK37" s="1"/>
     </row>
     <row r="38" spans="1:89" x14ac:dyDescent="0.2">
@@ -10856,6 +10971,9 @@
       <c r="CF38" s="4">
         <v>168.36277579999998</v>
       </c>
+      <c r="CG38" s="7">
+        <v>7744.9260545999996</v>
+      </c>
       <c r="CK38" s="1"/>
     </row>
     <row r="39" spans="1:89" x14ac:dyDescent="0.2">
@@ -11111,6 +11229,9 @@
       <c r="CF39" s="4">
         <v>158.15009090000001</v>
       </c>
+      <c r="CG39" s="7">
+        <v>7738.5979183999998</v>
+      </c>
       <c r="CK39" s="1"/>
     </row>
     <row r="40" spans="1:89" x14ac:dyDescent="0.2">
@@ -11366,6 +11487,9 @@
       <c r="CF40" s="4">
         <v>157.88430990000001</v>
       </c>
+      <c r="CG40" s="7">
+        <v>7857.9087863000004</v>
+      </c>
       <c r="CK40" s="1"/>
     </row>
     <row r="41" spans="1:89" x14ac:dyDescent="0.2">
@@ -11621,6 +11745,9 @@
       <c r="CF41" s="4">
         <v>166.52481809999998</v>
       </c>
+      <c r="CG41" s="7">
+        <v>7861.6938744999998</v>
+      </c>
       <c r="CK41" s="1"/>
     </row>
     <row r="42" spans="1:89" x14ac:dyDescent="0.2">
@@ -11876,6 +12003,9 @@
       <c r="CF42" s="4">
         <v>180.23433169999998</v>
       </c>
+      <c r="CG42" s="7">
+        <v>8003.2533721999998</v>
+      </c>
       <c r="CK42" s="1"/>
     </row>
     <row r="43" spans="1:89" x14ac:dyDescent="0.2">
@@ -12131,6 +12261,9 @@
       <c r="CF43" s="4">
         <v>176.95012789999998</v>
       </c>
+      <c r="CG43" s="7">
+        <v>8049.8759320999998</v>
+      </c>
       <c r="CK43" s="1"/>
     </row>
     <row r="44" spans="1:89" x14ac:dyDescent="0.2">
@@ -12386,6 +12519,9 @@
       <c r="CF44" s="4">
         <v>173.98325579999999</v>
       </c>
+      <c r="CG44" s="7">
+        <v>8165.2016004999996</v>
+      </c>
       <c r="CK44" s="1"/>
     </row>
     <row r="45" spans="1:89" x14ac:dyDescent="0.2">
@@ -12641,6 +12777,9 @@
       <c r="CF45" s="4">
         <v>173.98111550000002</v>
       </c>
+      <c r="CG45" s="7">
+        <v>8165.9187173999999</v>
+      </c>
       <c r="CK45" s="1"/>
     </row>
     <row r="46" spans="1:89" x14ac:dyDescent="0.2">
@@ -12896,6 +13035,9 @@
       <c r="CF46" s="4">
         <v>196.13978760000001</v>
       </c>
+      <c r="CG46" s="7">
+        <v>8300.2621098</v>
+      </c>
       <c r="CK46" s="1"/>
     </row>
     <row r="47" spans="1:89" x14ac:dyDescent="0.2">
@@ -13151,6 +13293,9 @@
       <c r="CF47" s="4">
         <v>192.53967270000001</v>
       </c>
+      <c r="CG47" s="7">
+        <v>8246.6034779000001</v>
+      </c>
       <c r="CK47" s="1"/>
     </row>
     <row r="48" spans="1:89" x14ac:dyDescent="0.2">
@@ -13406,6 +13551,9 @@
       <c r="CF48" s="4">
         <v>190.30363370000001</v>
       </c>
+      <c r="CG48" s="7">
+        <v>8297.1254308000007</v>
+      </c>
       <c r="CK48" s="1"/>
     </row>
     <row r="49" spans="1:89" x14ac:dyDescent="0.2">
@@ -13661,6 +13809,9 @@
       <c r="CF49" s="4">
         <v>173.44185920000001</v>
       </c>
+      <c r="CG49" s="7">
+        <v>8265.8648565000003</v>
+      </c>
       <c r="CK49" s="1"/>
     </row>
     <row r="50" spans="1:89" x14ac:dyDescent="0.2">
@@ -13916,6 +14067,9 @@
       <c r="CF50" s="4">
         <v>182.15074470000002</v>
       </c>
+      <c r="CG50" s="7">
+        <v>8314.3698521999995</v>
+      </c>
       <c r="CK50" s="1"/>
     </row>
     <row r="51" spans="1:89" x14ac:dyDescent="0.2">
@@ -14171,6 +14325,9 @@
       <c r="CF51" s="4">
         <v>182.872208</v>
       </c>
+      <c r="CG51" s="7">
+        <v>8291.3875501999992</v>
+      </c>
       <c r="CK51" s="1"/>
     </row>
     <row r="52" spans="1:89" x14ac:dyDescent="0.2">
@@ -14426,6 +14583,9 @@
       <c r="CF52" s="4">
         <v>187.7856305</v>
       </c>
+      <c r="CG52" s="7">
+        <v>8330.1864401999992</v>
+      </c>
       <c r="CK52" s="1"/>
     </row>
     <row r="53" spans="1:89" x14ac:dyDescent="0.2">
@@ -14681,6 +14841,9 @@
       <c r="CF53" s="4">
         <v>185.9952543</v>
       </c>
+      <c r="CG53" s="7">
+        <v>8250.3060526000008</v>
+      </c>
       <c r="CK53" s="1"/>
     </row>
     <row r="54" spans="1:89" x14ac:dyDescent="0.2">
@@ -14936,6 +15099,9 @@
       <c r="CF54" s="4">
         <v>194.65869990000002</v>
       </c>
+      <c r="CG54" s="7">
+        <v>8462.0847288000004</v>
+      </c>
       <c r="CK54" s="1"/>
     </row>
     <row r="55" spans="1:89" x14ac:dyDescent="0.2">
@@ -15191,6 +15357,9 @@
       <c r="CF55" s="4">
         <v>192.0231014</v>
       </c>
+      <c r="CG55" s="7">
+        <v>8412.9965838999997</v>
+      </c>
       <c r="CK55" s="1"/>
     </row>
     <row r="56" spans="1:89" x14ac:dyDescent="0.2">
@@ -15446,6 +15615,9 @@
       <c r="CF56" s="4">
         <v>189.16447980000001</v>
       </c>
+      <c r="CG56" s="7">
+        <v>8482.5400183999991</v>
+      </c>
       <c r="CK56" s="1"/>
     </row>
     <row r="57" spans="1:89" x14ac:dyDescent="0.2">
@@ -15701,6 +15873,9 @@
       <c r="CF57" s="4">
         <v>184.65895089999998</v>
       </c>
+      <c r="CG57" s="7">
+        <v>8455.2334644000002</v>
+      </c>
       <c r="CK57" s="1"/>
     </row>
     <row r="58" spans="1:89" x14ac:dyDescent="0.2">
@@ -15956,6 +16131,9 @@
       <c r="CF58" s="4">
         <v>195.62882640000001</v>
       </c>
+      <c r="CG58" s="7">
+        <v>8554.2948639000006</v>
+      </c>
       <c r="CK58" s="1"/>
     </row>
     <row r="59" spans="1:89" x14ac:dyDescent="0.2">
@@ -16211,6 +16389,9 @@
       <c r="CF59" s="4">
         <v>186.6266397</v>
       </c>
+      <c r="CG59" s="7">
+        <v>8556.4741814999998</v>
+      </c>
       <c r="CK59" s="1"/>
     </row>
     <row r="60" spans="1:89" x14ac:dyDescent="0.2">
@@ -16466,6 +16647,9 @@
       <c r="CF60" s="4">
         <v>181.31369709999998</v>
       </c>
+      <c r="CG60" s="7">
+        <v>8606.5201228000005</v>
+      </c>
       <c r="CK60" s="1"/>
     </row>
     <row r="61" spans="1:89" x14ac:dyDescent="0.2">
@@ -16721,6 +16905,9 @@
       <c r="CF61" s="4">
         <v>186.7026401</v>
       </c>
+      <c r="CG61" s="7">
+        <v>8603.6235892000004</v>
+      </c>
       <c r="CK61" s="1"/>
     </row>
     <row r="62" spans="1:89" x14ac:dyDescent="0.2">
@@ -16976,6 +17163,9 @@
       <c r="CF62" s="4">
         <v>190.6105359</v>
       </c>
+      <c r="CG62" s="7">
+        <v>8763.6674767999993</v>
+      </c>
       <c r="CK62" s="1"/>
     </row>
     <row r="63" spans="1:89" x14ac:dyDescent="0.2">
@@ -17231,6 +17421,9 @@
       <c r="CF63" s="4">
         <v>191.6836739</v>
       </c>
+      <c r="CG63" s="7">
+        <v>8754.4042205000005</v>
+      </c>
       <c r="CK63" s="1"/>
     </row>
     <row r="64" spans="1:89" x14ac:dyDescent="0.2">
@@ -17486,6 +17679,9 @@
       <c r="CF64" s="4">
         <v>183.77093730000001</v>
       </c>
+      <c r="CG64" s="7">
+        <v>8864.9997810999994</v>
+      </c>
       <c r="CK64" s="1"/>
     </row>
     <row r="65" spans="1:89" x14ac:dyDescent="0.2">
@@ -17741,6 +17937,9 @@
       <c r="CF65" s="4">
         <v>171.99186110000002</v>
       </c>
+      <c r="CG65" s="7">
+        <v>8911.5878905000009</v>
+      </c>
       <c r="CK65" s="1"/>
     </row>
     <row r="66" spans="1:89" x14ac:dyDescent="0.2">
@@ -17996,6 +18195,9 @@
       <c r="CF66" s="4">
         <v>173.35137079999998</v>
       </c>
+      <c r="CG66" s="7">
+        <v>8912.7194727000006</v>
+      </c>
       <c r="CK66" s="1"/>
     </row>
     <row r="67" spans="1:89" x14ac:dyDescent="0.2">
@@ -18251,6 +18453,9 @@
       <c r="CF67" s="4">
         <v>187.15537169999999</v>
       </c>
+      <c r="CG67" s="7">
+        <v>8920.9354323999996</v>
+      </c>
       <c r="CK67" s="1"/>
     </row>
     <row r="68" spans="1:89" x14ac:dyDescent="0.2">
@@ -18506,6 +18711,9 @@
       <c r="CF68" s="4">
         <v>202.24448240000001</v>
       </c>
+      <c r="CG68" s="7">
+        <v>9004.6291142999999</v>
+      </c>
       <c r="CK68" s="1"/>
     </row>
     <row r="69" spans="1:89" x14ac:dyDescent="0.2">
@@ -18761,6 +18969,9 @@
       <c r="CF69" s="4">
         <v>204.37893629999999</v>
       </c>
+      <c r="CG69" s="7">
+        <v>8971.8953963000004</v>
+      </c>
       <c r="CK69" s="1"/>
     </row>
     <row r="70" spans="1:89" x14ac:dyDescent="0.2">
@@ -19016,6 +19227,9 @@
       <c r="CF70" s="4">
         <v>203.66946329999999</v>
       </c>
+      <c r="CG70" s="7">
+        <v>9055.6440251000004</v>
+      </c>
       <c r="CK70" s="1"/>
     </row>
     <row r="71" spans="1:89" x14ac:dyDescent="0.2">
@@ -19271,6 +19485,9 @@
       <c r="CF71" s="4">
         <v>183.278257</v>
       </c>
+      <c r="CG71" s="7">
+        <v>9092.3099364999998</v>
+      </c>
       <c r="CK71" s="1"/>
     </row>
     <row r="72" spans="1:89" x14ac:dyDescent="0.2">
@@ -19526,6 +19743,9 @@
       <c r="CF72" s="4">
         <v>189.10933320000001</v>
       </c>
+      <c r="CG72" s="7">
+        <v>9134.6730812999995</v>
+      </c>
       <c r="CK72" s="1"/>
     </row>
     <row r="73" spans="1:89" x14ac:dyDescent="0.2">
@@ -19781,6 +20001,9 @@
       <c r="CF73" s="4">
         <v>206.23931709999999</v>
       </c>
+      <c r="CG73" s="7">
+        <v>9150.2861487999999</v>
+      </c>
       <c r="CK73" s="1"/>
     </row>
     <row r="74" spans="1:89" x14ac:dyDescent="0.2">
@@ -20036,6 +20259,9 @@
       <c r="CF74" s="4">
         <v>206.01434840000002</v>
       </c>
+      <c r="CG74" s="7">
+        <v>9286.7409043999996</v>
+      </c>
       <c r="CK74" s="1"/>
     </row>
     <row r="75" spans="1:89" x14ac:dyDescent="0.2">
@@ -20291,6 +20517,9 @@
       <c r="CF75" s="4">
         <v>210.2949362</v>
       </c>
+      <c r="CG75" s="7">
+        <v>9372.5993873000007</v>
+      </c>
       <c r="CK75" s="1"/>
     </row>
     <row r="76" spans="1:89" x14ac:dyDescent="0.2">
@@ -20546,6 +20775,9 @@
       <c r="CF76" s="4">
         <v>203.9154632</v>
       </c>
+      <c r="CG76" s="7">
+        <v>9380.0778465999992</v>
+      </c>
       <c r="CK76" s="1"/>
     </row>
     <row r="77" spans="1:89" x14ac:dyDescent="0.2">
@@ -20801,6 +21033,9 @@
       <c r="CF77" s="4">
         <v>200.81349889999998</v>
       </c>
+      <c r="CG77" s="7">
+        <v>9326.9510515999991</v>
+      </c>
       <c r="CK77" s="1"/>
     </row>
     <row r="78" spans="1:89" x14ac:dyDescent="0.2">
@@ -21056,6 +21291,9 @@
       <c r="CF78" s="4">
         <v>193.21786689999999</v>
       </c>
+      <c r="CG78" s="7">
+        <v>9427.7396370000006</v>
+      </c>
       <c r="CK78" s="1"/>
     </row>
     <row r="79" spans="1:89" x14ac:dyDescent="0.2">
@@ -21311,6 +21549,9 @@
       <c r="CF79" s="4">
         <v>201.4945869</v>
       </c>
+      <c r="CG79" s="7">
+        <v>9434.4538051</v>
+      </c>
       <c r="CK79" s="1"/>
     </row>
     <row r="80" spans="1:89" x14ac:dyDescent="0.2">
@@ -21566,6 +21807,9 @@
       <c r="CF80" s="4">
         <v>204.58887440000001</v>
       </c>
+      <c r="CG80" s="7">
+        <v>9533.4733240000005</v>
+      </c>
       <c r="CK80" s="1"/>
     </row>
     <row r="81" spans="1:89" x14ac:dyDescent="0.2">
@@ -21821,6 +22065,9 @@
       <c r="CF81" s="4">
         <v>211.46257840000001</v>
       </c>
+      <c r="CG81" s="7">
+        <v>9462.0865529000002</v>
+      </c>
       <c r="CK81" s="1"/>
     </row>
     <row r="82" spans="1:89" x14ac:dyDescent="0.2">
@@ -22076,6 +22323,9 @@
       <c r="CF82" s="4">
         <v>193.06659740000001</v>
       </c>
+      <c r="CG82" s="7">
+        <v>9652.9227023999993</v>
+      </c>
       <c r="CK82" s="1"/>
     </row>
     <row r="83" spans="1:89" x14ac:dyDescent="0.2">
@@ -22331,6 +22581,9 @@
       <c r="CF83" s="4">
         <v>191.66718349999999</v>
       </c>
+      <c r="CG83" s="7">
+        <v>9744.6145959999994</v>
+      </c>
       <c r="CK83" s="1"/>
     </row>
     <row r="84" spans="1:89" x14ac:dyDescent="0.2">
@@ -22586,6 +22839,9 @@
       <c r="CF84" s="4">
         <v>194.9898264</v>
       </c>
+      <c r="CG84" s="7">
+        <v>9850.7550761000002</v>
+      </c>
       <c r="CK84" s="1"/>
     </row>
     <row r="85" spans="1:89" x14ac:dyDescent="0.2">
@@ -22841,6 +23097,9 @@
       <c r="CF85" s="4">
         <v>201.8446452</v>
       </c>
+      <c r="CG85" s="7">
+        <v>9870.3355114000005</v>
+      </c>
       <c r="CK85" s="1"/>
     </row>
     <row r="86" spans="1:89" x14ac:dyDescent="0.2">
@@ -23096,6 +23355,9 @@
       <c r="CF86" s="4">
         <v>196.5723514</v>
       </c>
+      <c r="CG86" s="7">
+        <v>9944.9981674999999</v>
+      </c>
       <c r="CK86" s="1"/>
     </row>
     <row r="87" spans="1:89" x14ac:dyDescent="0.2">
@@ -23351,6 +23613,9 @@
       <c r="CF87" s="4">
         <v>202.25627060000002</v>
       </c>
+      <c r="CG87" s="7">
+        <v>9961.1373913999996</v>
+      </c>
       <c r="CK87" s="1"/>
     </row>
     <row r="88" spans="1:89" x14ac:dyDescent="0.2">
@@ -23606,6 +23871,9 @@
       <c r="CF88" s="4">
         <v>210.68401890000001</v>
       </c>
+      <c r="CG88" s="7">
+        <v>10082.055874600001</v>
+      </c>
       <c r="CK88" s="1"/>
     </row>
     <row r="89" spans="1:89" x14ac:dyDescent="0.2">
@@ -23861,6 +24129,9 @@
       <c r="CF89" s="4">
         <v>196.01130000000001</v>
       </c>
+      <c r="CG89" s="7">
+        <v>10105.7732289</v>
+      </c>
       <c r="CK89" s="1"/>
     </row>
     <row r="90" spans="1:89" x14ac:dyDescent="0.2">
@@ -24116,6 +24387,9 @@
       <c r="CF90" s="4">
         <v>203.6466317</v>
       </c>
+      <c r="CG90" s="7">
+        <v>10201.645047</v>
+      </c>
       <c r="CK90" s="1"/>
     </row>
     <row r="91" spans="1:89" x14ac:dyDescent="0.2">
@@ -24371,6 +24645,9 @@
       <c r="CF91" s="4">
         <v>206.81579090000002</v>
       </c>
+      <c r="CG91" s="7">
+        <v>10276.9833392</v>
+      </c>
       <c r="CK91" s="1"/>
     </row>
     <row r="92" spans="1:89" x14ac:dyDescent="0.2">
@@ -24626,6 +24903,9 @@
       <c r="CF92" s="4">
         <v>209.80413179999999</v>
       </c>
+      <c r="CG92" s="7">
+        <v>10412.0073436</v>
+      </c>
       <c r="CK92" s="1"/>
     </row>
     <row r="93" spans="1:89" x14ac:dyDescent="0.2">
@@ -24881,6 +25161,9 @@
       <c r="CF93" s="4">
         <v>211.7808928</v>
       </c>
+      <c r="CG93" s="7">
+        <v>10406.3975414</v>
+      </c>
       <c r="CK93" s="1"/>
     </row>
     <row r="94" spans="1:89" x14ac:dyDescent="0.2">
@@ -25136,6 +25419,9 @@
       <c r="CF94" s="4">
         <v>248.60622739999999</v>
       </c>
+      <c r="CG94" s="7">
+        <v>10535.100047800001</v>
+      </c>
       <c r="CK94" s="1"/>
     </row>
     <row r="95" spans="1:89" x14ac:dyDescent="0.2">
@@ -25391,6 +25677,9 @@
       <c r="CF95" s="4">
         <v>235.63359829999999</v>
       </c>
+      <c r="CG95" s="7">
+        <v>10622.906644500001</v>
+      </c>
       <c r="CK95" s="1"/>
     </row>
     <row r="96" spans="1:89" x14ac:dyDescent="0.2">
@@ -25646,6 +25935,9 @@
       <c r="CF96" s="4">
         <v>234.39561120000002</v>
       </c>
+      <c r="CG96" s="7">
+        <v>10690.3063561</v>
+      </c>
       <c r="CK96" s="1"/>
     </row>
     <row r="97" spans="1:89" x14ac:dyDescent="0.2">
@@ -25901,6 +26193,9 @@
       <c r="CF97" s="4">
         <v>222.25263420000002</v>
       </c>
+      <c r="CG97" s="7">
+        <v>10710.441137600001</v>
+      </c>
       <c r="CK97" s="1"/>
     </row>
     <row r="98" spans="1:89" x14ac:dyDescent="0.2">
@@ -26156,6 +26451,9 @@
       <c r="CF98" s="4">
         <v>220.20496439999999</v>
       </c>
+      <c r="CG98" s="7">
+        <v>10757.3446362</v>
+      </c>
       <c r="CK98" s="1"/>
     </row>
     <row r="99" spans="1:89" x14ac:dyDescent="0.2">
@@ -26411,6 +26709,9 @@
       <c r="CF99" s="4">
         <v>223.88401290000002</v>
       </c>
+      <c r="CG99" s="7">
+        <v>10776.7288095</v>
+      </c>
       <c r="CK99" s="1"/>
     </row>
     <row r="100" spans="1:89" x14ac:dyDescent="0.2">
@@ -26666,6 +26967,9 @@
       <c r="CF100" s="4">
         <v>221.95091689999998</v>
       </c>
+      <c r="CG100" s="7">
+        <v>10786.7987139</v>
+      </c>
       <c r="CK100" s="1"/>
     </row>
     <row r="101" spans="1:89" x14ac:dyDescent="0.2">
@@ -26921,6 +27225,9 @@
       <c r="CF101" s="4">
         <v>225.94482439999999</v>
       </c>
+      <c r="CG101" s="7">
+        <v>10707.257287500001</v>
+      </c>
       <c r="CK101" s="1"/>
     </row>
     <row r="102" spans="1:89" x14ac:dyDescent="0.2">
@@ -27176,6 +27483,9 @@
       <c r="CF102" s="4">
         <v>229.7956772</v>
       </c>
+      <c r="CG102" s="7">
+        <v>10829.231529500001</v>
+      </c>
       <c r="CK102" s="1"/>
     </row>
     <row r="103" spans="1:89" x14ac:dyDescent="0.2">
@@ -27431,6 +27741,9 @@
       <c r="CF103" s="4">
         <v>235.44695249999998</v>
       </c>
+      <c r="CG103" s="7">
+        <v>10889.154493399999</v>
+      </c>
       <c r="CK103" s="1"/>
     </row>
     <row r="104" spans="1:89" x14ac:dyDescent="0.2">
@@ -27686,6 +27999,9 @@
       <c r="CF104" s="4">
         <v>225.9643902</v>
       </c>
+      <c r="CG104" s="7">
+        <v>10957.4266088</v>
+      </c>
       <c r="CK104" s="1"/>
     </row>
     <row r="105" spans="1:89" x14ac:dyDescent="0.2">
@@ -27941,6 +28257,9 @@
       <c r="CF105" s="4">
         <v>209.45087580000001</v>
       </c>
+      <c r="CG105" s="7">
+        <v>10973.8229331</v>
+      </c>
       <c r="CK105" s="1"/>
     </row>
     <row r="106" spans="1:89" x14ac:dyDescent="0.2">
@@ -28196,6 +28515,9 @@
       <c r="CF106" s="4">
         <v>233.53403390000003</v>
       </c>
+      <c r="CG106" s="7">
+        <v>11144.5452391</v>
+      </c>
       <c r="CK106" s="1"/>
     </row>
     <row r="107" spans="1:89" x14ac:dyDescent="0.2">
@@ -28451,6 +28773,9 @@
       <c r="CF107" s="4">
         <v>214.5775256</v>
       </c>
+      <c r="CG107" s="7">
+        <v>11146.1760954</v>
+      </c>
       <c r="CK107" s="1"/>
     </row>
     <row r="108" spans="1:89" x14ac:dyDescent="0.2">
@@ -28706,6 +29031,9 @@
       <c r="CF108" s="4">
         <v>214.0277959</v>
       </c>
+      <c r="CG108" s="7">
+        <v>11196.181066900001</v>
+      </c>
       <c r="CK108" s="1"/>
     </row>
     <row r="109" spans="1:89" x14ac:dyDescent="0.2">
@@ -28961,6 +29289,9 @@
       <c r="CF109" s="4">
         <v>214.80691400000001</v>
       </c>
+      <c r="CG109" s="7">
+        <v>11127.2154885</v>
+      </c>
       <c r="CK109" s="1"/>
     </row>
     <row r="110" spans="1:89" x14ac:dyDescent="0.2">
@@ -29216,6 +29547,9 @@
       <c r="CF110" s="4">
         <v>227.31274820000002</v>
       </c>
+      <c r="CG110" s="7">
+        <v>11239.4184518</v>
+      </c>
       <c r="CK110" s="1"/>
     </row>
     <row r="111" spans="1:89" x14ac:dyDescent="0.2">
@@ -29471,6 +29805,9 @@
       <c r="CF111" s="4">
         <v>246.5488149</v>
       </c>
+      <c r="CG111" s="7">
+        <v>11237.735913099999</v>
+      </c>
       <c r="CK111" s="1"/>
     </row>
     <row r="112" spans="1:89" x14ac:dyDescent="0.2">
@@ -29726,6 +30063,9 @@
       <c r="CF112" s="4">
         <v>239.2303311</v>
       </c>
+      <c r="CG112" s="7">
+        <v>11393.152977899999</v>
+      </c>
       <c r="CK112" s="1"/>
     </row>
     <row r="113" spans="1:89" x14ac:dyDescent="0.2">
@@ -29981,6 +30321,9 @@
       <c r="CF113" s="4">
         <v>228.13694090000001</v>
       </c>
+      <c r="CG113" s="7">
+        <v>11264.1168555</v>
+      </c>
       <c r="CK113" s="1"/>
     </row>
     <row r="114" spans="1:89" x14ac:dyDescent="0.2">
@@ -30236,6 +30579,9 @@
       <c r="CF114" s="4">
         <v>233.2491675</v>
       </c>
+      <c r="CG114" s="7">
+        <v>11378.3335893</v>
+      </c>
       <c r="CK114" s="1"/>
     </row>
     <row r="115" spans="1:89" x14ac:dyDescent="0.2">
@@ -30491,6 +30837,9 @@
       <c r="CF115" s="4">
         <v>223.0060478</v>
       </c>
+      <c r="CG115" s="7">
+        <v>11425.3118584</v>
+      </c>
       <c r="CK115" s="1"/>
     </row>
     <row r="116" spans="1:89" x14ac:dyDescent="0.2">
@@ -30746,6 +31095,9 @@
       <c r="CF116" s="4">
         <v>240.16123540000001</v>
       </c>
+      <c r="CG116" s="7">
+        <v>11491.664766399999</v>
+      </c>
       <c r="CK116" s="1"/>
     </row>
     <row r="117" spans="1:89" x14ac:dyDescent="0.2">
@@ -31001,6 +31353,9 @@
       <c r="CF117" s="4">
         <v>252.71318069999998</v>
       </c>
+      <c r="CG117" s="7">
+        <v>11361.409787299999</v>
+      </c>
       <c r="CK117" s="1"/>
     </row>
     <row r="118" spans="1:89" x14ac:dyDescent="0.2">
@@ -31256,6 +31611,9 @@
       <c r="CF118" s="4">
         <v>252.98245929999999</v>
       </c>
+      <c r="CG118" s="7">
+        <v>11445.9000442</v>
+      </c>
       <c r="CK118" s="1"/>
     </row>
     <row r="119" spans="1:89" x14ac:dyDescent="0.2">
@@ -31511,6 +31869,9 @@
       <c r="CF119" s="4">
         <v>239.5790293</v>
       </c>
+      <c r="CG119" s="7">
+        <v>11464.564434100001</v>
+      </c>
       <c r="CK119" s="1"/>
     </row>
     <row r="120" spans="1:89" x14ac:dyDescent="0.2">
@@ -31766,6 +32127,9 @@
       <c r="CF120" s="4">
         <v>259.14199990000003</v>
       </c>
+      <c r="CG120" s="7">
+        <v>11553.348763100001</v>
+      </c>
       <c r="CK120" s="1"/>
     </row>
     <row r="121" spans="1:89" x14ac:dyDescent="0.2">
@@ -32021,6 +32385,9 @@
       <c r="CF121" s="4">
         <v>242.62766980000001</v>
       </c>
+      <c r="CG121" s="7">
+        <v>11572.7635314</v>
+      </c>
       <c r="CK121" s="1"/>
     </row>
     <row r="122" spans="1:89" x14ac:dyDescent="0.2">
@@ -32276,6 +32643,9 @@
       <c r="CF122" s="4">
         <v>246.8317692</v>
       </c>
+      <c r="CG122" s="7">
+        <v>11581.725704</v>
+      </c>
       <c r="CK122" s="1"/>
     </row>
     <row r="123" spans="1:89" x14ac:dyDescent="0.2">
@@ -32531,6 +32901,9 @@
       <c r="CF123" s="4">
         <v>253.85951489999999</v>
       </c>
+      <c r="CG123" s="7">
+        <v>11724.132317</v>
+      </c>
       <c r="CK123" s="1"/>
     </row>
     <row r="124" spans="1:89" x14ac:dyDescent="0.2">
@@ -32786,6 +33159,9 @@
       <c r="CF124" s="4">
         <v>252.21548050000001</v>
       </c>
+      <c r="CG124" s="7">
+        <v>11781.440931200001</v>
+      </c>
       <c r="CK124" s="1"/>
     </row>
     <row r="125" spans="1:89" x14ac:dyDescent="0.2">
@@ -33041,6 +33417,9 @@
       <c r="CF125" s="4">
         <v>235.08123750000001</v>
       </c>
+      <c r="CG125" s="7">
+        <v>11702.631254899999</v>
+      </c>
       <c r="CK125" s="1"/>
     </row>
     <row r="126" spans="1:89" x14ac:dyDescent="0.2">
@@ -33296,6 +33675,9 @@
       <c r="CF126" s="4">
         <v>238.72651390000001</v>
       </c>
+      <c r="CG126" s="7">
+        <v>11935.266320000001</v>
+      </c>
       <c r="CK126" s="1"/>
     </row>
     <row r="127" spans="1:89" x14ac:dyDescent="0.2">
@@ -33551,6 +33933,9 @@
       <c r="CF127" s="4">
         <v>248.68904620000001</v>
       </c>
+      <c r="CG127" s="7">
+        <v>11975.894034499999</v>
+      </c>
       <c r="CK127" s="1"/>
     </row>
     <row r="128" spans="1:89" x14ac:dyDescent="0.2">
@@ -33806,6 +34191,9 @@
       <c r="CF128" s="4">
         <v>257.07791700000001</v>
       </c>
+      <c r="CG128" s="7">
+        <v>11999.9494196</v>
+      </c>
       <c r="CK128" s="1"/>
     </row>
     <row r="129" spans="1:89" x14ac:dyDescent="0.2">
@@ -34061,6 +34449,9 @@
       <c r="CF129" s="4">
         <v>274.10497200000003</v>
       </c>
+      <c r="CG129" s="7">
+        <v>11904.7089265</v>
+      </c>
       <c r="CK129" s="1"/>
     </row>
     <row r="130" spans="1:89" x14ac:dyDescent="0.2">
@@ -34316,6 +34707,9 @@
       <c r="CF130" s="4">
         <v>263.27242649999999</v>
       </c>
+      <c r="CG130" s="7">
+        <v>12054.006582399999</v>
+      </c>
       <c r="CK130" s="1"/>
     </row>
     <row r="131" spans="1:89" x14ac:dyDescent="0.2">
@@ -34571,6 +34965,9 @@
       <c r="CF131" s="4">
         <v>262.61110789999998</v>
       </c>
+      <c r="CG131" s="7">
+        <v>12103.333139</v>
+      </c>
       <c r="CK131" s="1"/>
     </row>
     <row r="132" spans="1:89" x14ac:dyDescent="0.2">
@@ -34826,6 +35223,9 @@
       <c r="CF132" s="4">
         <v>278.93157389999999</v>
       </c>
+      <c r="CG132" s="7">
+        <v>12256.6339114</v>
+      </c>
       <c r="CK132" s="1"/>
     </row>
     <row r="133" spans="1:89" x14ac:dyDescent="0.2">
@@ -35081,6 +35481,9 @@
       <c r="CF133" s="4">
         <v>271.0524891</v>
       </c>
+      <c r="CG133" s="7">
+        <v>12245.332033999999</v>
+      </c>
       <c r="CK133" s="1"/>
     </row>
     <row r="134" spans="1:89" x14ac:dyDescent="0.2">
@@ -35336,6 +35739,9 @@
       <c r="CF134" s="4">
         <v>280.41483060000002</v>
       </c>
+      <c r="CG134" s="7">
+        <v>12453.6309795</v>
+      </c>
       <c r="CK134" s="1"/>
     </row>
     <row r="135" spans="1:89" x14ac:dyDescent="0.2">
@@ -35591,6 +35997,9 @@
       <c r="CF135" s="4">
         <v>251.3279311</v>
       </c>
+      <c r="CG135" s="7">
+        <v>12528.1846948</v>
+      </c>
       <c r="CK135" s="1"/>
     </row>
     <row r="136" spans="1:89" x14ac:dyDescent="0.2">
@@ -35846,6 +36255,9 @@
       <c r="CF136" s="4">
         <v>251.88561010000001</v>
       </c>
+      <c r="CG136" s="7">
+        <v>12572.697362000001</v>
+      </c>
       <c r="CK136" s="1"/>
     </row>
     <row r="137" spans="1:89" x14ac:dyDescent="0.2">
@@ -36101,6 +36513,9 @@
       <c r="CF137" s="4">
         <v>266.70027210000001</v>
       </c>
+      <c r="CG137" s="7">
+        <v>12547.5377006</v>
+      </c>
       <c r="CK137" s="1"/>
     </row>
     <row r="138" spans="1:89" x14ac:dyDescent="0.2">
@@ -36356,6 +36771,9 @@
       <c r="CF138" s="4">
         <v>260.71605520000003</v>
       </c>
+      <c r="CG138" s="7">
+        <v>12741.586741900001</v>
+      </c>
       <c r="CK138" s="1"/>
     </row>
     <row r="139" spans="1:89" x14ac:dyDescent="0.2">
@@ -36611,6 +37029,9 @@
       <c r="CF139" s="4">
         <v>294.20246689999999</v>
       </c>
+      <c r="CG139" s="7">
+        <v>12802.157754600001</v>
+      </c>
       <c r="CK139" s="1"/>
     </row>
     <row r="140" spans="1:89" x14ac:dyDescent="0.2">
@@ -36866,6 +37287,9 @@
       <c r="CF140" s="4">
         <v>293.30516979999999</v>
       </c>
+      <c r="CG140" s="7">
+        <v>12921.060775899999</v>
+      </c>
       <c r="CK140" s="1"/>
     </row>
     <row r="141" spans="1:89" x14ac:dyDescent="0.2">
@@ -37121,6 +37545,9 @@
       <c r="CF141" s="4">
         <v>276.17982870000003</v>
       </c>
+      <c r="CG141" s="7">
+        <v>12858.8226376</v>
+      </c>
       <c r="CK141" s="1"/>
     </row>
     <row r="142" spans="1:89" x14ac:dyDescent="0.2">
@@ -37376,6 +37803,9 @@
       <c r="CF142" s="4">
         <v>280.50974479999996</v>
       </c>
+      <c r="CG142" s="7">
+        <v>12996.176518099999</v>
+      </c>
       <c r="CK142" s="1"/>
     </row>
     <row r="143" spans="1:89" x14ac:dyDescent="0.2">
@@ -37631,6 +38061,9 @@
       <c r="CF143" s="4">
         <v>251.81843320000002</v>
       </c>
+      <c r="CG143" s="7">
+        <v>13053.282018100001</v>
+      </c>
       <c r="CK143" s="1"/>
     </row>
     <row r="144" spans="1:89" x14ac:dyDescent="0.2">
@@ -37886,6 +38319,9 @@
       <c r="CF144" s="4">
         <v>225.52434910000002</v>
       </c>
+      <c r="CG144" s="7">
+        <v>12192.5802874</v>
+      </c>
       <c r="CK144" s="1"/>
     </row>
     <row r="145" spans="1:89" x14ac:dyDescent="0.2">
@@ -38141,6 +38577,9 @@
       <c r="CF145" s="4">
         <v>226.45940159999998</v>
       </c>
+      <c r="CG145" s="7">
+        <v>12562.7918001</v>
+      </c>
       <c r="CK145" s="1"/>
     </row>
     <row r="146" spans="1:89" x14ac:dyDescent="0.2">
@@ -38396,6 +38835,9 @@
       <c r="CF146" s="4">
         <v>246.11089630000001</v>
       </c>
+      <c r="CG146" s="7">
+        <v>12882.160213700001</v>
+      </c>
       <c r="CK146" s="1"/>
     </row>
     <row r="147" spans="1:89" x14ac:dyDescent="0.2">
@@ -38651,6 +39093,9 @@
       <c r="CF147" s="4">
         <v>282.34339650000004</v>
       </c>
+      <c r="CG147" s="7">
+        <v>13037.041243600001</v>
+      </c>
       <c r="CK147" s="1"/>
     </row>
     <row r="148" spans="1:89" x14ac:dyDescent="0.2">
@@ -38906,6 +39351,9 @@
       <c r="CF148" s="4">
         <v>296.98251099999999</v>
       </c>
+      <c r="CG148" s="7">
+        <v>13204.3429452</v>
+      </c>
       <c r="CK148" s="1"/>
     </row>
     <row r="149" spans="1:89" x14ac:dyDescent="0.2">
@@ -39161,6 +39609,9 @@
       <c r="CF149" s="4">
         <v>282.03680030000004</v>
       </c>
+      <c r="CG149" s="7">
+        <v>12955.3726811</v>
+      </c>
       <c r="CK149" s="1"/>
     </row>
     <row r="150" spans="1:89" x14ac:dyDescent="0.2">
@@ -39416,6 +39867,9 @@
       <c r="CF150" s="4">
         <v>290.7564443</v>
       </c>
+      <c r="CG150" s="7">
+        <v>13273.977877699999</v>
+      </c>
       <c r="CK150" s="1"/>
     </row>
     <row r="151" spans="1:89" x14ac:dyDescent="0.2">
@@ -39671,6 +40125,9 @@
       <c r="CF151" s="4">
         <v>275.94076039999999</v>
       </c>
+      <c r="CG151" s="7">
+        <v>13482.1191734</v>
+      </c>
       <c r="CK151" s="1"/>
     </row>
     <row r="152" spans="1:89" x14ac:dyDescent="0.2">
@@ -39925,6 +40382,9 @@
       </c>
       <c r="CF152" s="4">
         <v>302.11678940000002</v>
+      </c>
+      <c r="CG152" s="7">
+        <v>13589.1047423</v>
       </c>
     </row>
     <row r="153" spans="1:89" x14ac:dyDescent="0.2">

</xml_diff>